<commit_message>
updated log in uniquerowsfromcolumn xaml and resolved the error in UpdatColumnBasedOnOtherColumn xaml by adding the item column in excel
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sachin\Documents\UiPath\Pratice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAB857E-6CDF-48DA-BE3D-21A44DD860B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AECAA1B2-D1F5-41CA-92C9-26E232284866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="79">
   <si>
     <t>Company Name</t>
   </si>
@@ -1103,10 +1103,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F68"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1118,7 +1118,7 @@
     <col min="5" max="5" width="13.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1137,8 +1137,11 @@
       <c r="F1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1158,7 +1161,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1178,7 +1181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1198,7 +1201,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1218,7 +1221,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1238,7 +1241,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -1258,7 +1261,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1278,7 +1281,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1298,7 +1301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -1318,7 +1321,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -1338,7 +1341,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -1358,7 +1361,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -1378,7 +1381,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -1398,7 +1401,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2246,11 +2249,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{482BC2FF-04FE-48EF-86AC-967706E5ACB6}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:F41"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D46" sqref="D46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2263,7 +2265,7 @@
     <col min="6" max="6" width="5.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2280,10 +2282,13 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2299,8 +2304,11 @@
       <c r="E2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2316,8 +2324,11 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F3">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -2333,8 +2344,11 @@
       <c r="E4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -2350,8 +2364,11 @@
       <c r="E5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -2367,8 +2384,11 @@
       <c r="E6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -2384,11 +2404,14 @@
       <c r="E7" t="s">
         <v>28</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7">
+        <v>26</v>
+      </c>
+      <c r="G7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -2404,8 +2427,11 @@
       <c r="E8" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F8">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -2421,8 +2447,11 @@
       <c r="E9" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -2438,8 +2467,11 @@
       <c r="E10" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F10">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
@@ -2455,28 +2487,11 @@
       <c r="E11" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F11">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2492,8 +2507,11 @@
       <c r="E13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F13">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>48</v>
       </c>
@@ -2509,8 +2527,11 @@
       <c r="E14" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F14">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>52</v>
       </c>
@@ -2526,8 +2547,11 @@
       <c r="E15" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -2543,476 +2567,875 @@
       <c r="E16" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
-      </c>
-      <c r="E17" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F16">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
       <c r="C18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>31</v>
+      </c>
+      <c r="G18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" t="s">
+        <v>51</v>
+      </c>
+      <c r="F20">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>52</v>
+      </c>
+      <c r="B21" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D21" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" t="s">
+        <v>55</v>
+      </c>
+      <c r="F21">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" t="s">
+        <v>60</v>
+      </c>
+      <c r="D23" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>61</v>
+      </c>
+      <c r="F23">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>62</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="D18" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+      <c r="E24" t="s">
         <v>64</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F24">
+        <v>37</v>
+      </c>
+      <c r="G24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>65</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C25" t="s">
         <v>66</v>
       </c>
-      <c r="D19" t="s">
-        <v>8</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="D25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" t="s">
         <v>67</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F25">
+        <v>38</v>
+      </c>
+      <c r="G25" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
         <v>68</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B30" t="s">
         <v>69</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C30" t="s">
         <v>70</v>
       </c>
-      <c r="D20" t="s">
-        <v>8</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="D30" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="F30">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>72</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C31" t="s">
         <v>73</v>
       </c>
-      <c r="D21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="D31" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" t="s">
         <v>74</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F31">
+        <v>40</v>
+      </c>
+      <c r="G31" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>5</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B32" t="s">
         <v>6</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C32" t="s">
         <v>7</v>
       </c>
-      <c r="D22" t="s">
-        <v>77</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="D32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E32" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="F32">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>10</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B33" t="s">
         <v>11</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C33" t="s">
         <v>12</v>
       </c>
-      <c r="D23" t="s">
-        <v>77</v>
-      </c>
-      <c r="E23" t="s">
+      <c r="D33" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
+      <c r="F33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>14</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B34" t="s">
         <v>15</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C34" t="s">
         <v>16</v>
       </c>
-      <c r="D24" t="s">
-        <v>77</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="D34" t="s">
+        <v>77</v>
+      </c>
+      <c r="E34" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
+      <c r="F34">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>18</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C35" t="s">
         <v>19</v>
       </c>
-      <c r="D25" t="s">
-        <v>77</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="D35" t="s">
+        <v>77</v>
+      </c>
+      <c r="E35" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
+      <c r="F35">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>21</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B36" t="s">
         <v>22</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C36" t="s">
         <v>23</v>
       </c>
-      <c r="D26" t="s">
-        <v>77</v>
-      </c>
-      <c r="E26" t="s">
+      <c r="D36" t="s">
+        <v>77</v>
+      </c>
+      <c r="E36" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
+      <c r="F36">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B37" t="s">
         <v>26</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C37" t="s">
         <v>27</v>
       </c>
-      <c r="D27" t="s">
-        <v>77</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="D37" t="s">
+        <v>77</v>
+      </c>
+      <c r="E37" t="s">
         <v>28</v>
       </c>
-      <c r="F27" t="s">
+      <c r="F37">
+        <v>46</v>
+      </c>
+      <c r="G37" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>29</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C38" t="s">
         <v>30</v>
       </c>
-      <c r="D28" t="s">
-        <v>77</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="D38" t="s">
+        <v>77</v>
+      </c>
+      <c r="E38" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
+      <c r="F38">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
         <v>32</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B39" t="s">
         <v>33</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C39" t="s">
         <v>34</v>
       </c>
-      <c r="D29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="D39" t="s">
+        <v>77</v>
+      </c>
+      <c r="E39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
+      <c r="F39">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>36</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B40" t="s">
         <v>15</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C40" t="s">
         <v>37</v>
       </c>
-      <c r="D30" t="s">
-        <v>77</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="D40" t="s">
+        <v>77</v>
+      </c>
+      <c r="E40" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
+      <c r="F40">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B41" t="s">
         <v>15</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C41" t="s">
         <v>40</v>
       </c>
-      <c r="D31" t="s">
-        <v>77</v>
-      </c>
-      <c r="E31" t="s">
+      <c r="D41" t="s">
+        <v>77</v>
+      </c>
+      <c r="E41" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
+      <c r="F41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
         <v>42</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B42" t="s">
         <v>26</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C42" t="s">
         <v>43</v>
       </c>
-      <c r="D32" t="s">
-        <v>77</v>
-      </c>
-      <c r="E32" t="s">
+      <c r="D42" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" t="s">
         <v>44</v>
       </c>
-      <c r="F32" t="s">
+      <c r="F42">
+        <v>51</v>
+      </c>
+      <c r="G42" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>45</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B43" t="s">
         <v>33</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C43" t="s">
         <v>46</v>
       </c>
-      <c r="D33" t="s">
-        <v>77</v>
-      </c>
-      <c r="E33" t="s">
+      <c r="D43" t="s">
+        <v>77</v>
+      </c>
+      <c r="E43" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
+      <c r="F43">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>48</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B47" t="s">
         <v>49</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C47" t="s">
         <v>50</v>
       </c>
-      <c r="D34" t="s">
-        <v>77</v>
-      </c>
-      <c r="E34" t="s">
+      <c r="D47" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+      <c r="F47">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>52</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B48" t="s">
         <v>53</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C48" t="s">
         <v>54</v>
       </c>
-      <c r="D35" t="s">
-        <v>77</v>
-      </c>
-      <c r="E35" t="s">
+      <c r="D48" t="s">
+        <v>77</v>
+      </c>
+      <c r="E48" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
+      <c r="F48">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>56</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B49" t="s">
         <v>11</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C49" t="s">
         <v>57</v>
       </c>
-      <c r="D36" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="D49" t="s">
+        <v>77</v>
+      </c>
+      <c r="E49" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="F49">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>59</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B50" t="s">
         <v>53</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C50" t="s">
         <v>60</v>
       </c>
-      <c r="D37" t="s">
-        <v>77</v>
-      </c>
-      <c r="E37" t="s">
+      <c r="D50" t="s">
+        <v>77</v>
+      </c>
+      <c r="E50" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="F50">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>62</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B51" t="s">
         <v>26</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C51" t="s">
         <v>63</v>
       </c>
-      <c r="D38" t="s">
-        <v>77</v>
-      </c>
-      <c r="E38" t="s">
+      <c r="D51" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" t="s">
         <v>64</v>
       </c>
-      <c r="F38" t="s">
+      <c r="F51">
+        <v>57</v>
+      </c>
+      <c r="G51" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>65</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B52" t="s">
         <v>26</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C52" t="s">
         <v>66</v>
       </c>
-      <c r="D39" t="s">
-        <v>77</v>
-      </c>
-      <c r="E39" t="s">
+      <c r="D52" t="s">
+        <v>77</v>
+      </c>
+      <c r="E52" t="s">
         <v>67</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F52">
+        <v>58</v>
+      </c>
+      <c r="G52" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>68</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B53" t="s">
         <v>69</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C53" t="s">
         <v>70</v>
       </c>
-      <c r="D40" t="s">
-        <v>77</v>
-      </c>
-      <c r="E40" t="s">
+      <c r="D53" t="s">
+        <v>77</v>
+      </c>
+      <c r="E53" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+      <c r="F53">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>72</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B54" t="s">
         <v>26</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C54" t="s">
         <v>73</v>
       </c>
-      <c r="D41" t="s">
-        <v>77</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="D54" t="s">
+        <v>77</v>
+      </c>
+      <c r="E54" t="s">
         <v>74</v>
       </c>
-      <c r="F41" t="s">
+      <c r="F54">
+        <v>60</v>
+      </c>
+      <c r="G54" t="s">
         <v>76</v>
       </c>
     </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" t="s">
+        <v>15</v>
+      </c>
+      <c r="C58" t="s">
+        <v>37</v>
+      </c>
+      <c r="D58" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>39</v>
+      </c>
+      <c r="B59" t="s">
+        <v>15</v>
+      </c>
+      <c r="C59" t="s">
+        <v>40</v>
+      </c>
+      <c r="D59" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" t="s">
+        <v>41</v>
+      </c>
+      <c r="F59">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" t="s">
+        <v>26</v>
+      </c>
+      <c r="C60" t="s">
+        <v>43</v>
+      </c>
+      <c r="D60" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" t="s">
+        <v>44</v>
+      </c>
+      <c r="F60">
+        <v>31</v>
+      </c>
+      <c r="G60" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>45</v>
+      </c>
+      <c r="B61" t="s">
+        <v>33</v>
+      </c>
+      <c r="C61" t="s">
+        <v>46</v>
+      </c>
+      <c r="D61" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" t="s">
+        <v>47</v>
+      </c>
+      <c r="F61">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>48</v>
+      </c>
+      <c r="B62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C62" t="s">
+        <v>50</v>
+      </c>
+      <c r="D62" t="s">
+        <v>8</v>
+      </c>
+      <c r="E62" t="s">
+        <v>51</v>
+      </c>
+      <c r="F62">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>52</v>
+      </c>
+      <c r="B63" t="s">
+        <v>53</v>
+      </c>
+      <c r="C63" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" t="s">
+        <v>8</v>
+      </c>
+      <c r="E63" t="s">
+        <v>55</v>
+      </c>
+      <c r="F63">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64" t="s">
+        <v>11</v>
+      </c>
+      <c r="C64" t="s">
+        <v>57</v>
+      </c>
+      <c r="D64" t="s">
+        <v>8</v>
+      </c>
+      <c r="E64" t="s">
+        <v>58</v>
+      </c>
+      <c r="F64">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>59</v>
+      </c>
+      <c r="B65" t="s">
+        <v>53</v>
+      </c>
+      <c r="C65" t="s">
+        <v>60</v>
+      </c>
+      <c r="D65" t="s">
+        <v>8</v>
+      </c>
+      <c r="E65" t="s">
+        <v>61</v>
+      </c>
+      <c r="F65">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>62</v>
+      </c>
+      <c r="B66" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" t="s">
+        <v>8</v>
+      </c>
+      <c r="E66" t="s">
+        <v>64</v>
+      </c>
+      <c r="F66">
+        <v>37</v>
+      </c>
+      <c r="G66" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" t="s">
+        <v>8</v>
+      </c>
+      <c r="E67" t="s">
+        <v>67</v>
+      </c>
+      <c r="F67">
+        <v>38</v>
+      </c>
+      <c r="G67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>69</v>
+      </c>
+      <c r="C68" t="s">
+        <v>70</v>
+      </c>
+      <c r="D68" t="s">
+        <v>8</v>
+      </c>
+      <c r="E68" t="s">
+        <v>71</v>
+      </c>
+      <c r="F68">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F41" xr:uid="{482BC2FF-04FE-48EF-86AC-967706E5ACB6}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Information Technology"/>
-      </filters>
-    </filterColumn>
-    <filterColumn colId="3">
-      <filters>
-        <filter val="FQ"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F41" xr:uid="{482BC2FF-04FE-48EF-86AC-967706E5ACB6}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65CE730C-EAC0-4553-BC03-2DC9D6583ED9}">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
@@ -3073,11 +3496,6 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>42</v>
-      </c>
-    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>45</v>
@@ -3100,26 +3518,31 @@
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>72</v>
       </c>
     </row>

</xml_diff>